<commit_message>
Fixed small typo in QB MOOC v1 parts list.
</commit_message>
<xml_diff>
--- a/robots/quickbot/mooc/v1/quickbot_parts_v1.xlsx
+++ b/robots/quickbot/mooc/v1/quickbot_parts_v1.xlsx
@@ -33,9 +33,6 @@
     <t>BeagleBone Black</t>
   </si>
   <si>
-    <t>Quanity</t>
-  </si>
-  <si>
     <t>Motor Controller</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>Octopart</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1368,14 +1367,14 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="11" style="29" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
@@ -1386,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="28">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="7"/>
@@ -1411,44 +1410,44 @@
         <v>2</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>4</v>
+        <v>155</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="40" t="s">
-        <v>115</v>
-      </c>
       <c r="H3" s="40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="37" customFormat="1" ht="20">
       <c r="C4" s="38"/>
       <c r="D4" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1">
@@ -1461,10 +1460,10 @@
     </row>
     <row r="6" spans="1:9" s="12" customFormat="1">
       <c r="A6" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="26">
         <v>1</v>
@@ -1484,16 +1483,16 @@
         <v>5.29</v>
       </c>
       <c r="H6" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1">
       <c r="A7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="C7" s="26">
         <v>1</v>
@@ -1513,16 +1512,16 @@
         <v>12.95</v>
       </c>
       <c r="H7" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:9" s="12" customFormat="1">
       <c r="A8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="C8" s="26">
         <v>1</v>
@@ -1542,18 +1541,18 @@
         <v>1.55</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="12" customFormat="1">
       <c r="A9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="C9" s="26">
         <v>1</v>
@@ -1573,18 +1572,18 @@
         <v>0.09</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="12" customFormat="1">
       <c r="A10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="C10" s="26">
         <v>1</v>
@@ -1604,16 +1603,16 @@
         <v>0.08</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" s="12" customFormat="1">
       <c r="A11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="C11" s="26">
         <v>1</v>
@@ -1633,18 +1632,18 @@
         <v>0.1</v>
       </c>
       <c r="H11" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1">
       <c r="A12" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="26">
         <v>1</v>
@@ -1664,18 +1663,18 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="12" customFormat="1">
       <c r="A13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C13" s="26">
         <v>7</v>
@@ -1695,18 +1694,18 @@
         <v>0.42</v>
       </c>
       <c r="H13" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="12" customFormat="1">
       <c r="A14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="C14" s="26">
         <v>7</v>
@@ -1726,10 +1725,10 @@
         <v>0.42</v>
       </c>
       <c r="H14" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="12" customFormat="1">
@@ -1757,18 +1756,18 @@
         <v>40.455000000000005</v>
       </c>
       <c r="H15" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="12" customFormat="1">
       <c r="A16" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="26">
         <v>2</v>
@@ -1788,18 +1787,18 @@
         <v>5.4</v>
       </c>
       <c r="H16" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="12" customFormat="1">
       <c r="A17" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="26">
         <v>1</v>
@@ -1819,15 +1818,15 @@
         <v>2.25</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="12" customFormat="1">
       <c r="A18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="C18" s="26">
         <v>1</v>
@@ -1847,15 +1846,15 @@
         <v>13.455</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1">
       <c r="A19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="C19" s="26">
         <v>1</v>
@@ -1875,18 +1874,18 @@
         <v>9</v>
       </c>
       <c r="H19" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="12" customFormat="1">
       <c r="A20" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="26">
         <v>1</v>
@@ -1906,18 +1905,18 @@
         <v>3.5550000000000002</v>
       </c>
       <c r="H20" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="12" customFormat="1">
       <c r="A21" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="26">
         <v>1</v>
@@ -1937,15 +1936,15 @@
         <v>4.4550000000000001</v>
       </c>
       <c r="H21" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="12" customFormat="1">
       <c r="A22" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="26">
         <v>1</v>
@@ -1965,15 +1964,15 @@
         <v>3.5550000000000002</v>
       </c>
       <c r="H22" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="12" customFormat="1">
       <c r="A23" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="26">
         <v>2</v>
@@ -1993,15 +1992,15 @@
         <v>2.7</v>
       </c>
       <c r="H23" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="12" customFormat="1">
       <c r="A24" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="26">
         <v>2</v>
@@ -2021,15 +2020,15 @@
         <v>2.7</v>
       </c>
       <c r="H24" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="12" customFormat="1">
       <c r="A25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="C25" s="26">
         <v>2</v>
@@ -2049,15 +2048,15 @@
         <v>2.7</v>
       </c>
       <c r="H25" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="12" customFormat="1">
       <c r="A26" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="26">
         <v>1</v>
@@ -2077,18 +2076,18 @@
         <v>2.1150000000000002</v>
       </c>
       <c r="H26" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="12" customFormat="1">
       <c r="A27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="C27" s="26">
         <v>1</v>
@@ -2108,18 +2107,18 @@
         <v>0.81</v>
       </c>
       <c r="H27" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="12" customFormat="1">
       <c r="A28" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="26">
         <v>1</v>
@@ -2139,15 +2138,15 @@
         <v>0.85499999999999998</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="12" customFormat="1">
       <c r="A29" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="26">
         <v>5</v>
@@ -2167,18 +2166,18 @@
         <v>63</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="12" customFormat="1">
       <c r="A30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="C30" s="26">
         <v>5</v>
@@ -2198,15 +2197,15 @@
         <v>6.75</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="12" customFormat="1">
       <c r="A31" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="C31" s="26">
         <v>10</v>
@@ -2226,7 +2225,7 @@
         <v>4.05</v>
       </c>
       <c r="H31" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="12" customFormat="1">
@@ -2239,7 +2238,7 @@
     </row>
     <row r="33" spans="1:8" s="17" customFormat="1" ht="20">
       <c r="A33" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="27">
         <f>SUM(C29:C31)</f>
@@ -2264,7 +2263,7 @@
     </row>
     <row r="35" spans="1:8" s="41" customFormat="1" ht="20">
       <c r="A35" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="43"/>
@@ -2283,10 +2282,10 @@
     </row>
     <row r="37" spans="1:8" s="12" customFormat="1">
       <c r="A37" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="31" t="s">
         <v>103</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>104</v>
       </c>
       <c r="C37" s="32">
         <v>1</v>
@@ -2305,15 +2304,15 @@
         <v>18.170000000000002</v>
       </c>
       <c r="H37" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="12" customFormat="1">
       <c r="A38" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="34">
         <v>1</v>
@@ -2332,7 +2331,7 @@
         <v>9.99</v>
       </c>
       <c r="H38" s="48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="12" customFormat="1">
@@ -2345,7 +2344,7 @@
     </row>
     <row r="40" spans="1:8" s="17" customFormat="1" ht="20">
       <c r="A40" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" s="27">
         <f>SUM(C37:C38)</f>
@@ -2370,7 +2369,7 @@
     </row>
     <row r="42" spans="1:8" s="41" customFormat="1" ht="20">
       <c r="A42" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43"/>
@@ -2389,10 +2388,10 @@
     </row>
     <row r="44" spans="1:8" s="12" customFormat="1">
       <c r="A44" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="26">
         <v>1</v>
@@ -2412,15 +2411,15 @@
         <v>4</v>
       </c>
       <c r="H44" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="12" customFormat="1">
       <c r="A45" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="26">
         <v>1</v>
@@ -2440,15 +2439,15 @@
         <v>9</v>
       </c>
       <c r="H45" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="12" customFormat="1">
       <c r="A46" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="26">
         <v>1</v>
@@ -2468,15 +2467,15 @@
         <v>4</v>
       </c>
       <c r="H46" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="12" customFormat="1">
       <c r="A47" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" s="26">
         <v>1</v>
@@ -2496,15 +2495,15 @@
         <v>6.5</v>
       </c>
       <c r="H47" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="12" customFormat="1">
       <c r="A48" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="26">
         <v>1</v>
@@ -2524,7 +2523,7 @@
         <v>0.85499999999999998</v>
       </c>
       <c r="H48" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="12" customFormat="1">
@@ -2537,7 +2536,7 @@
     </row>
     <row r="50" spans="1:9" s="17" customFormat="1" ht="20">
       <c r="A50" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="27">
         <f>SUM(C44:C48)</f>
@@ -2562,7 +2561,7 @@
     </row>
     <row r="52" spans="1:9" s="41" customFormat="1" ht="20">
       <c r="A52" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C52" s="42"/>
       <c r="D52" s="43"/>
@@ -2581,10 +2580,10 @@
     </row>
     <row r="54" spans="1:9" s="12" customFormat="1">
       <c r="A54" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="C54" s="26">
         <v>1</v>
@@ -2604,18 +2603,18 @@
         <v>6.5</v>
       </c>
       <c r="H54" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="12" customFormat="1">
       <c r="A55" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55" s="26">
         <v>1</v>
@@ -2635,18 +2634,18 @@
         <v>5.3550000000000004</v>
       </c>
       <c r="H55" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="12" customFormat="1">
       <c r="A56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="C56" s="26">
         <v>1</v>
@@ -2666,18 +2665,18 @@
         <v>6.95</v>
       </c>
       <c r="H56" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="12" customFormat="1">
       <c r="A57" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="C57" s="26">
         <v>1</v>
@@ -2697,15 +2696,15 @@
         <v>1.55</v>
       </c>
       <c r="H57" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="12" customFormat="1">
       <c r="A58" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>125</v>
       </c>
       <c r="C58" s="26">
         <v>1</v>
@@ -2725,18 +2724,18 @@
         <v>0.68400000000000005</v>
       </c>
       <c r="H58" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="12" customFormat="1">
       <c r="A59" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="C59" s="26">
         <v>1</v>
@@ -2756,15 +2755,15 @@
         <v>1.46</v>
       </c>
       <c r="H59" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="12" customFormat="1">
       <c r="A60" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="C60" s="26">
         <v>1</v>
@@ -2784,7 +2783,7 @@
         <v>10.314000000000002</v>
       </c>
       <c r="H60" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="12" customFormat="1">
@@ -2797,7 +2796,7 @@
     </row>
     <row r="62" spans="1:9" s="17" customFormat="1" ht="20">
       <c r="A62" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C62" s="27">
         <f>SUM(C54:C61)</f>
@@ -2814,7 +2813,7 @@
     </row>
     <row r="64" spans="1:9" s="41" customFormat="1" ht="20">
       <c r="A64" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C64" s="42"/>
       <c r="D64" s="43"/>
@@ -2833,10 +2832,10 @@
     </row>
     <row r="66" spans="1:9" s="12" customFormat="1">
       <c r="A66" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="C66" s="26">
         <v>1</v>
@@ -2856,7 +2855,7 @@
         <v>14.95</v>
       </c>
       <c r="H66" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="12" customFormat="1">
@@ -2884,18 +2883,18 @@
         <v>45</v>
       </c>
       <c r="H67" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="12" customFormat="1">
       <c r="A68" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C68" s="26">
         <v>1</v>
@@ -2915,18 +2914,18 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="H68" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="12" customFormat="1">
       <c r="A69" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="C69" s="26">
         <v>2</v>
@@ -2946,18 +2945,18 @@
         <v>3.9</v>
       </c>
       <c r="H69" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="12" customFormat="1">
       <c r="A70" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="12" t="s">
         <v>6</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>7</v>
       </c>
       <c r="C70" s="26">
         <v>2</v>
@@ -2977,18 +2976,18 @@
         <v>8</v>
       </c>
       <c r="H70" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="12" customFormat="1">
       <c r="A71" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C71" s="32">
         <v>1</v>
@@ -3008,15 +3007,15 @@
         <v>5.69</v>
       </c>
       <c r="H71" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="12" customFormat="1">
       <c r="A72" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C72" s="26">
         <v>1</v>
@@ -3036,18 +3035,18 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="H72" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="12" customFormat="1">
       <c r="A73" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C73" s="26">
         <v>1</v>
@@ -3067,18 +3066,18 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="H73" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="12" customFormat="1">
       <c r="A74" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C74" s="26">
         <v>1</v>
@@ -3098,18 +3097,18 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="H74" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="12" customFormat="1">
       <c r="A75" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C75" s="26">
         <v>1</v>
@@ -3129,18 +3128,18 @@
         <v>0.315</v>
       </c>
       <c r="H75" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="12" customFormat="1">
       <c r="A76" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="C76" s="26">
         <v>2</v>
@@ -3160,15 +3159,15 @@
         <v>7.11</v>
       </c>
       <c r="H76" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="12" customFormat="1">
       <c r="A77" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" s="26">
         <v>1</v>
@@ -3188,15 +3187,15 @@
         <v>4.4550000000000001</v>
       </c>
       <c r="H77" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="12" customFormat="1">
       <c r="A78" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="C78" s="26">
         <v>8</v>
@@ -3216,15 +3215,15 @@
         <v>3.6</v>
       </c>
       <c r="H78" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="12" customFormat="1">
       <c r="A79" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C79" s="26">
         <v>1</v>
@@ -3244,15 +3243,15 @@
         <v>6.16</v>
       </c>
       <c r="H79" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="12" customFormat="1">
       <c r="A80" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="C80" s="26">
         <v>1</v>
@@ -3272,15 +3271,15 @@
         <v>0.46</v>
       </c>
       <c r="H80" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="12" customFormat="1">
       <c r="A81" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C81" s="26">
         <v>1</v>
@@ -3300,15 +3299,15 @@
         <v>11.25</v>
       </c>
       <c r="H81" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="12" customFormat="1">
       <c r="A82" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="C82" s="26">
         <v>1</v>
@@ -3328,15 +3327,15 @@
         <v>8</v>
       </c>
       <c r="H82" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="12" customFormat="1">
       <c r="A83" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" s="26">
         <v>1</v>
@@ -3356,10 +3355,10 @@
         <v>7.95</v>
       </c>
       <c r="H83" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I83" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>